<commit_message>
feat: add new ecModels
</commit_message>
<xml_diff>
--- a/result_ecYeast/Data_Allchemicals.xlsx
+++ b/result_ecYeast/Data_Allchemicals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="3HP_Rxn " sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Models!$E$1:$E$97</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4035" uniqueCount="3006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4317" uniqueCount="3210">
   <si>
     <t>3-hydroxypropionate dehydrogenase</t>
   </si>
@@ -15337,6 +15337,1119 @@
   </si>
   <si>
     <t>s_4402 -&gt;</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miltiradiene</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0373No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0190 + s_0943 + 4.20875e-05 prot_Q12051 -&gt; s_0189 + s_0633 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.6 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00044 mmol/gDCW/h</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00053 mmol/gDCW/h</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEP</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTS1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modular Pathway Engineering of Diterpenoid Synthases and the Mevalonic Acid Pathway for Miltiradiene Production</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0355No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0943 + s_1376 + 0.000126263 prot_P08524  -&gt; s_0633 + s_0745 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5.1.1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0462No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0745 + s_0943 + 0.000126263 prot_P08524  -&gt; s_0190 + s_0633 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0558No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">pmet_r_0558 + 3.0013e-06 prot_P12684  -&gt; s_0028 + s_0529 + 2 s_1207 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1.1.34</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>92.5526 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>HMG1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>labdadienyl/copalyl diphosphate synthase</t>
+  </si>
+  <si>
+    <t>s_0189 + prot_B8PQ84 -&gt; s_4403</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CPS (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Salvia miltiorrhiza</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>B8PQ84</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.5.1.12</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>kaurene synthase</t>
+  </si>
+  <si>
+    <t>s_4403 + prot_C8XPS0 -&gt; s_0633 + s_4404</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KSL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Salvia miltiorrhiza</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>C8XPS0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.3.131</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miltiradiene transport</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4404 -&gt; s_4405</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miltiradiene exchange</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_4405 -&gt; </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_B8PQ84</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>90.483 prot_pool  -&gt; prot_B8PQ84</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_C8XPS0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>68.37 prot_pool  -&gt; prot_C8XPS0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4403[c]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copalyl diphosphate [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4404[c]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miltiradiene [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4405[e]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miltiradiene [extracellular]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4405[e]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miltiradiene [extracellular]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecMiltiradiene.mat</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>heterogenous</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Caffeic acid</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>coumarate 3-hydroxylase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4231 + prot_O22203 -&gt; s_4387</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>C3H (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Arabidopsis thaliana</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>O22203</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.14.13.-</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00029 g/g</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00033 g/g</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEP</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARO10, PDC5</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>De Novo Biosynthesis of Caffeic Acid from Glucose by Engineered Saccharomyces cerevisiae</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>tyrosine ammonia-lyase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_1051 + 1.00281e-05 prot_A0A1M4NET9 -&gt; s_0419 + s_4231</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>TAL (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rhodobacter capsulatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0A1M4NET9</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.3.1.23</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0551 + s_0803 + s_1360 + 0.0033548 prot_P32449ly  -&gt; s_0349 + s_1322 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>ARO4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K229L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S. cerevisiae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>P32449ly</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0515 + 0.00207452 prot_P32178ly  -&gt; s_1377 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>ARO7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>G141S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S. cerevisiae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>P32178ly</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.99.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_O22203</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>57.927 prot_pool  -&gt; prot_O22203</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_A0A1M4NET9</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>55.539 prot_pool  -&gt; prot_A0A1M4NET9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_P32449ly</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>39.7487 prot_pool  -&gt; prot_P32449ly</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_P32178ly</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>29.7468 prot_pool  -&gt; prot_P32178ly</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>caffeic acid transpory</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4387 -&gt; s_4406</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>caffeic acid exchange</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4406 -&gt;</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>valencene synthase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_0190 + 0.0868056 prot_S4SC87 -&gt; s_4407 + s_0633</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>VS (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Callitropsis nootkatensis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>S4SC87</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.3.73</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.0032 mol/mol</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEP</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTS1, DPP1, LPP1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>High production of valencene in Saccharomyces cerevisiae through metabolic engineering</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>valencene transport</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4407 -&gt; s_4408</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>valencene exchange</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4408 -&gt;</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_S4SC87</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>69.219 prot_pool  -&gt; prot_S4SC87</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0558No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">pmet_r_0558 + 3.0013e-06 prot_P12684  -&gt; s_0028 + s_0529 + 2 s_1207 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1.1.34</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HMG1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0904No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0019 + s_0434 + 4.08497e-05 prot_P24521  -&gt; s_0018 + s_0394 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.7.4.2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.8 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERG8</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0103No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2 s_0373 + 1.54321e-07 prot_P41338  -&gt; s_0367 + s_0529 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3.1.9</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1800 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERG10</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0104No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2 s_0376 + 1.54321e-07 prot_P41338  -&gt; s_0370 + s_0532 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0103_REVNo1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0367 + s_0529 + 2.77778e-11 pprot_P41338  -&gt; 2 s_0373 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000000 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0104_REVNo1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0370 + s_0532 + 2.77778e-11 pprot_P41338  -&gt; 2 s_0376 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0735No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0028 + s_0434 + 6.34194e-06 prot_P07277  -&gt; s_0019 + s_0394 + s_0794 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.7.1.36</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>43.8001 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERG12</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0028 + s_0539 + 6.34194e-06 prot_P07277  -&gt; s_0019 + s_0467 + s_0794 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0028 + s_0785 + 6.34194e-06 prot_P07277  -&gt; s_0019 + s_0739 + s_0794 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0028 + s_1559 + 6.34194e-06 prot_P07277  -&gt; s_0019 + s_0794 + s_1538 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0559No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0367 + s_0373 + s_0803 + 0.000334672 prot_P54839  -&gt; s_0218 + s_0529 + s_0794 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3.3.10</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.83 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0370 + s_0376 + s_0807 + 0.000334672 prot_P54839  -&gt; s_0221 + s_0532 + s_0799 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0739No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0018 + s_0434 + 2.83447e-05 prot_P32377  -&gt; s_0394 + s_0456 + s_0943 + s_1322 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1.1.33</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.8 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERG19</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0355No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0943 + s_1376 + 0.000126263 prot_P08524  -&gt; s_0633 + s_0745 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5.1.1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0462No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0745 + s_0943 + 0.000126263 prot_P08524  -&gt; s_0190 + s_0633 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0667No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0943 + 4.64511e-09 prot_P15496  -&gt; s_1376 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.3.3.2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>59800 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDI1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0667_REVNo1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_1376 + 0.0022919 prot_P15496  -&gt; s_0943 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1212 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2 s_0190 + s_0794 + s_1212 + 0.0003367 prot_P29704  -&gt; 2 s_0633 + s_1207 + s_1447 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5.1.21</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERG9: downregulation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>β-amyrin synthase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_0037 + 0.00036075 prot_Q9MB42 -&gt; s_4272</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>bAS (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Glycyrrhiza glabra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q9MB42</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.99.39</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00017 mol/mol</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEP</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Controlling Chemo- and Regioselectivity of a Plant P450 in Yeast Cell toward Rare Licorice Triterpenoid Biosynthesis</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beta-amyrin 11-oxidase</t>
+  </si>
+  <si>
+    <t>s_4272 + 2 s_1275 + prot_A0A218KSA8 -&gt; s_4409 + 3 s_0803</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>uni25647 (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chinese licorice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0A218KSA8</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.14.14.152</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>11-oxo-beta-amyrin 30-oxidase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CYP72A63 (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medicago truncatula</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>H1A981</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.14.14.115</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glycyrrhetinic acid transport</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4410 -&gt; s_4411</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glycyrrhetinic acid exchange</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4411 -&gt;</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q9MB42</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>87.516 prot_pool  -&gt; prot_Q9MB42</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_A0A218KSA8</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>56.456 prot_pool  -&gt; prot_A0A218KSA8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_H1A981</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>59.454 prot_pool  -&gt; prot_H1A981</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glycyrrhetinic acid</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valencene</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4406[e]</t>
+  </si>
+  <si>
+    <t>caffeic acid [extracellular]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4407[c]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>valencene [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4408[e]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>valencene [extracellular]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4409[c]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>11-Oxo-beta-amyrin [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4410[c]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glycyrrhetinic acid [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4411[e]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glycyrrhetinic acid [extracellular]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecCaffeic_acid.mat</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>heterogenous</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecValencene.mat</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecGlycyrrhetinic_acid.mat</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4409 + 3 s_1275 + prot_H1A981 -&gt; s_4410 + 4 s_0803</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>glucose</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -17454,10 +18567,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T699"/>
+  <dimension ref="A1:T753"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A681" workbookViewId="0">
-      <selection activeCell="A682" sqref="A682:XFD699"/>
+    <sheetView tabSelected="1" topLeftCell="F673" workbookViewId="0">
+      <selection activeCell="N706" sqref="N706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -30959,7 +32072,7 @@
         <v>2983</v>
       </c>
     </row>
-    <row r="689" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="689" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B689" s="13">
         <v>8</v>
       </c>
@@ -30970,7 +32083,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="690" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="690" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B690" s="13">
         <v>9</v>
       </c>
@@ -30981,7 +32094,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="691" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="691" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B691" s="13">
         <v>10</v>
       </c>
@@ -30992,7 +32105,7 @@
         <v>2989</v>
       </c>
     </row>
-    <row r="692" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="692" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B692" s="13">
         <v>11</v>
       </c>
@@ -31003,7 +32116,7 @@
         <v>2991</v>
       </c>
     </row>
-    <row r="693" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="693" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B693" s="13">
         <v>12</v>
       </c>
@@ -31014,7 +32127,7 @@
         <v>2993</v>
       </c>
     </row>
-    <row r="694" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="694" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B694" s="13">
         <v>13</v>
       </c>
@@ -31025,7 +32138,7 @@
         <v>2995</v>
       </c>
     </row>
-    <row r="695" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="695" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B695" s="13">
         <v>14</v>
       </c>
@@ -31036,7 +32149,7 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="696" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="696" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B696" s="13">
         <v>15</v>
       </c>
@@ -31047,7 +32160,7 @@
         <v>2999</v>
       </c>
     </row>
-    <row r="697" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="697" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B697" s="13">
         <v>16</v>
       </c>
@@ -31058,7 +32171,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="698" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="698" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B698" s="13">
         <v>17</v>
       </c>
@@ -31069,7 +32182,7 @@
         <v>3003</v>
       </c>
     </row>
-    <row r="699" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="699" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B699" s="13">
         <v>18</v>
       </c>
@@ -31078,6 +32191,1095 @@
       </c>
       <c r="D699" s="2" t="s">
         <v>3005</v>
+      </c>
+    </row>
+    <row r="700" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B700" s="13"/>
+    </row>
+    <row r="701" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A701" s="2" t="s">
+        <v>3006</v>
+      </c>
+      <c r="B701" s="2" t="s">
+        <v>3007</v>
+      </c>
+      <c r="C701" s="2" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D701" s="2" t="s">
+        <v>3008</v>
+      </c>
+      <c r="E701" s="12"/>
+      <c r="F701" s="12"/>
+      <c r="G701" s="12"/>
+      <c r="H701" s="12" t="s">
+        <v>3009</v>
+      </c>
+      <c r="I701" s="12"/>
+      <c r="J701" s="12"/>
+      <c r="K701" s="12"/>
+      <c r="L701" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="M701" s="12" t="s">
+        <v>3010</v>
+      </c>
+      <c r="N701" s="12" t="s">
+        <v>3011</v>
+      </c>
+      <c r="O701" s="12" t="s">
+        <v>3012</v>
+      </c>
+      <c r="P701" s="12" t="s">
+        <v>3209</v>
+      </c>
+      <c r="Q701" s="12" t="s">
+        <v>3013</v>
+      </c>
+      <c r="S701" s="2" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="702" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B702" t="s">
+        <v>3015</v>
+      </c>
+      <c r="C702" t="s">
+        <v>875</v>
+      </c>
+      <c r="D702" t="s">
+        <v>3016</v>
+      </c>
+      <c r="E702" s="2"/>
+      <c r="F702" s="2"/>
+      <c r="G702" s="2" t="s">
+        <v>3017</v>
+      </c>
+      <c r="H702" s="12" t="s">
+        <v>3018</v>
+      </c>
+      <c r="I702" s="2">
+        <v>40.482900000000001</v>
+      </c>
+      <c r="J702" s="2"/>
+      <c r="K702" s="2"/>
+      <c r="L702" s="20"/>
+      <c r="M702" s="2"/>
+      <c r="N702" s="2"/>
+      <c r="O702" s="2"/>
+      <c r="P702" s="2"/>
+      <c r="Q702" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="703" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B703" t="s">
+        <v>3019</v>
+      </c>
+      <c r="C703" t="s">
+        <v>458</v>
+      </c>
+      <c r="D703" t="s">
+        <v>3020</v>
+      </c>
+      <c r="G703" s="2" t="s">
+        <v>3017</v>
+      </c>
+      <c r="H703" s="12" t="s">
+        <v>3018</v>
+      </c>
+      <c r="I703" s="2">
+        <v>40.482900000000001</v>
+      </c>
+      <c r="Q703" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="704" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B704" t="s">
+        <v>3021</v>
+      </c>
+      <c r="C704" t="s">
+        <v>370</v>
+      </c>
+      <c r="D704" t="s">
+        <v>3022</v>
+      </c>
+      <c r="E704" s="12"/>
+      <c r="F704" s="12"/>
+      <c r="G704" s="12" t="s">
+        <v>3023</v>
+      </c>
+      <c r="H704" s="12" t="s">
+        <v>3024</v>
+      </c>
+      <c r="I704" s="12">
+        <v>115.691</v>
+      </c>
+      <c r="J704" s="12"/>
+      <c r="K704" s="12"/>
+      <c r="L704" s="21"/>
+      <c r="M704" s="12"/>
+      <c r="N704" s="12"/>
+      <c r="O704" s="12"/>
+      <c r="P704" s="12"/>
+      <c r="Q704" s="12" t="s">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="705" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B705" s="2">
+        <v>1</v>
+      </c>
+      <c r="C705" s="2" t="s">
+        <v>3026</v>
+      </c>
+      <c r="D705" s="2" t="s">
+        <v>3027</v>
+      </c>
+      <c r="E705" s="2" t="s">
+        <v>3028</v>
+      </c>
+      <c r="F705" s="2" t="s">
+        <v>3029</v>
+      </c>
+      <c r="G705" s="12" t="s">
+        <v>3030</v>
+      </c>
+      <c r="H705" t="s">
+        <v>3031</v>
+      </c>
+      <c r="I705" s="12">
+        <v>90.483000000000004</v>
+      </c>
+    </row>
+    <row r="706" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B706" s="2">
+        <v>2</v>
+      </c>
+      <c r="C706" s="2" t="s">
+        <v>3032</v>
+      </c>
+      <c r="D706" s="2" t="s">
+        <v>3033</v>
+      </c>
+      <c r="E706" s="12" t="s">
+        <v>3034</v>
+      </c>
+      <c r="F706" s="2" t="s">
+        <v>3035</v>
+      </c>
+      <c r="G706" s="12" t="s">
+        <v>3036</v>
+      </c>
+      <c r="H706" t="s">
+        <v>3031</v>
+      </c>
+      <c r="I706">
+        <v>68.37</v>
+      </c>
+    </row>
+    <row r="707" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B707" s="2">
+        <v>3</v>
+      </c>
+      <c r="C707" s="2" t="s">
+        <v>3037</v>
+      </c>
+      <c r="D707" s="2" t="s">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="708" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B708" s="2">
+        <v>4</v>
+      </c>
+      <c r="C708" s="2" t="s">
+        <v>3039</v>
+      </c>
+      <c r="D708" s="2" t="s">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="709" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B709" s="2">
+        <v>5</v>
+      </c>
+      <c r="C709" s="12" t="s">
+        <v>3041</v>
+      </c>
+      <c r="D709" s="12" t="s">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="710" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B710" s="2">
+        <v>6</v>
+      </c>
+      <c r="C710" s="12" t="s">
+        <v>3043</v>
+      </c>
+      <c r="D710" s="12" t="s">
+        <v>3044</v>
+      </c>
+    </row>
+    <row r="712" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A712" s="2" t="s">
+        <v>3055</v>
+      </c>
+      <c r="B712" s="2">
+        <v>1</v>
+      </c>
+      <c r="C712" s="2" t="s">
+        <v>3056</v>
+      </c>
+      <c r="D712" s="2" t="s">
+        <v>3057</v>
+      </c>
+      <c r="E712" s="2" t="s">
+        <v>3058</v>
+      </c>
+      <c r="F712" s="2" t="s">
+        <v>3059</v>
+      </c>
+      <c r="G712" s="2" t="s">
+        <v>3060</v>
+      </c>
+      <c r="H712" s="2" t="s">
+        <v>3061</v>
+      </c>
+      <c r="I712" s="2">
+        <v>57.927</v>
+      </c>
+      <c r="L712" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="M712" s="2" t="s">
+        <v>3062</v>
+      </c>
+      <c r="N712" s="2" t="s">
+        <v>3063</v>
+      </c>
+      <c r="O712" s="2" t="s">
+        <v>3064</v>
+      </c>
+      <c r="P712" s="2" t="s">
+        <v>3209</v>
+      </c>
+      <c r="R712" s="2" t="s">
+        <v>3065</v>
+      </c>
+      <c r="S712" s="2" t="s">
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="713" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B713" s="13">
+        <v>2</v>
+      </c>
+      <c r="C713" s="12" t="s">
+        <v>3067</v>
+      </c>
+      <c r="D713" s="12" t="s">
+        <v>3068</v>
+      </c>
+      <c r="E713" s="12" t="s">
+        <v>3069</v>
+      </c>
+      <c r="F713" s="12" t="s">
+        <v>3070</v>
+      </c>
+      <c r="G713" s="12" t="s">
+        <v>3071</v>
+      </c>
+      <c r="H713" s="17">
+        <v>27.7</v>
+      </c>
+      <c r="I713" s="12">
+        <v>55.539000000000001</v>
+      </c>
+    </row>
+    <row r="714" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B714" s="8">
+        <v>3</v>
+      </c>
+      <c r="C714" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D714" s="2" t="s">
+        <v>3072</v>
+      </c>
+      <c r="E714" s="2" t="s">
+        <v>3073</v>
+      </c>
+      <c r="F714" s="2" t="s">
+        <v>3074</v>
+      </c>
+      <c r="G714" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H714" s="2">
+        <v>8.280979166666666E-2</v>
+      </c>
+      <c r="I714" s="2">
+        <v>39.748699999999999</v>
+      </c>
+      <c r="J714" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="K714" s="8"/>
+      <c r="L714" s="9"/>
+      <c r="M714" s="8"/>
+      <c r="S714" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="715" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A715" s="16"/>
+      <c r="B715" s="13">
+        <v>4</v>
+      </c>
+      <c r="C715" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="D715" s="12" t="s">
+        <v>3075</v>
+      </c>
+      <c r="E715" s="12" t="s">
+        <v>3076</v>
+      </c>
+      <c r="F715" s="12" t="s">
+        <v>3077</v>
+      </c>
+      <c r="G715" s="12" t="s">
+        <v>3078</v>
+      </c>
+      <c r="H715" s="12">
+        <v>0.13386060000000002</v>
+      </c>
+      <c r="I715" s="12">
+        <v>29.7468</v>
+      </c>
+      <c r="J715" s="12">
+        <v>0.27</v>
+      </c>
+      <c r="L715" s="21"/>
+    </row>
+    <row r="716" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B716" s="8">
+        <v>5</v>
+      </c>
+      <c r="C716" s="12" t="s">
+        <v>3079</v>
+      </c>
+      <c r="D716" s="12" t="s">
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="717" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B717" s="13">
+        <v>6</v>
+      </c>
+      <c r="C717" s="12" t="s">
+        <v>3081</v>
+      </c>
+      <c r="D717" s="12" t="s">
+        <v>3082</v>
+      </c>
+    </row>
+    <row r="718" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B718" s="8">
+        <v>7</v>
+      </c>
+      <c r="C718" s="12" t="s">
+        <v>3083</v>
+      </c>
+      <c r="D718" s="12" t="s">
+        <v>3084</v>
+      </c>
+    </row>
+    <row r="719" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B719" s="13">
+        <v>8</v>
+      </c>
+      <c r="C719" s="12" t="s">
+        <v>3085</v>
+      </c>
+      <c r="D719" s="12" t="s">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="720" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B720" s="8">
+        <v>9</v>
+      </c>
+      <c r="C720" s="12" t="s">
+        <v>3087</v>
+      </c>
+      <c r="D720" s="2" t="s">
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="721" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B721" s="13">
+        <v>10</v>
+      </c>
+      <c r="C721" s="2" t="s">
+        <v>3089</v>
+      </c>
+      <c r="D721" s="2" t="s">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="723" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A723" s="2" t="s">
+        <v>3191</v>
+      </c>
+      <c r="B723" s="13">
+        <v>1</v>
+      </c>
+      <c r="C723" s="2" t="s">
+        <v>3091</v>
+      </c>
+      <c r="D723" s="2" t="s">
+        <v>3092</v>
+      </c>
+      <c r="E723" s="2" t="s">
+        <v>3093</v>
+      </c>
+      <c r="F723" s="2" t="s">
+        <v>3094</v>
+      </c>
+      <c r="G723" s="2" t="s">
+        <v>3095</v>
+      </c>
+      <c r="H723" s="2">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="I723" s="2">
+        <v>69.218999999999994</v>
+      </c>
+      <c r="L723" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="N723" s="2" t="s">
+        <v>3096</v>
+      </c>
+      <c r="O723" s="2" t="s">
+        <v>3097</v>
+      </c>
+      <c r="P723" s="2" t="s">
+        <v>3209</v>
+      </c>
+      <c r="R723" s="2" t="s">
+        <v>3098</v>
+      </c>
+      <c r="S723" s="2" t="s">
+        <v>3099</v>
+      </c>
+    </row>
+    <row r="724" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B724" s="13">
+        <v>2</v>
+      </c>
+      <c r="C724" s="2" t="s">
+        <v>3100</v>
+      </c>
+      <c r="D724" s="2" t="s">
+        <v>3101</v>
+      </c>
+    </row>
+    <row r="725" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B725" s="13">
+        <v>3</v>
+      </c>
+      <c r="C725" s="2" t="s">
+        <v>3102</v>
+      </c>
+      <c r="D725" s="2" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="726" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B726" s="13">
+        <v>4</v>
+      </c>
+      <c r="C726" s="12" t="s">
+        <v>3104</v>
+      </c>
+      <c r="D726" s="12" t="s">
+        <v>3105</v>
+      </c>
+    </row>
+    <row r="727" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B727" t="s">
+        <v>3106</v>
+      </c>
+      <c r="C727" t="s">
+        <v>370</v>
+      </c>
+      <c r="D727" t="s">
+        <v>3107</v>
+      </c>
+      <c r="E727" s="12"/>
+      <c r="F727" s="12"/>
+      <c r="G727" s="12" t="s">
+        <v>3108</v>
+      </c>
+      <c r="H727" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="I727" s="12">
+        <v>115.691</v>
+      </c>
+      <c r="Q727" s="20" t="s">
+        <v>3109</v>
+      </c>
+    </row>
+    <row r="728" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B728" t="s">
+        <v>3110</v>
+      </c>
+      <c r="C728" t="s">
+        <v>846</v>
+      </c>
+      <c r="D728" t="s">
+        <v>3111</v>
+      </c>
+      <c r="G728" s="2" t="s">
+        <v>3112</v>
+      </c>
+      <c r="H728" s="12" t="s">
+        <v>3113</v>
+      </c>
+      <c r="I728" s="2">
+        <v>50.4544</v>
+      </c>
+      <c r="Q728" s="2" t="s">
+        <v>3114</v>
+      </c>
+    </row>
+    <row r="729" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B729" t="s">
+        <v>3115</v>
+      </c>
+      <c r="C729" t="s">
+        <v>850</v>
+      </c>
+      <c r="D729" t="s">
+        <v>3116</v>
+      </c>
+      <c r="G729" s="2" t="s">
+        <v>3117</v>
+      </c>
+      <c r="H729" s="12" t="s">
+        <v>3118</v>
+      </c>
+      <c r="I729" s="2">
+        <v>41.728200000000001</v>
+      </c>
+      <c r="Q729" s="2" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="730" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B730" t="s">
+        <v>3120</v>
+      </c>
+      <c r="C730" t="s">
+        <v>850</v>
+      </c>
+      <c r="D730" t="s">
+        <v>3121</v>
+      </c>
+      <c r="G730" s="2" t="s">
+        <v>3117</v>
+      </c>
+      <c r="H730" s="12" t="s">
+        <v>3118</v>
+      </c>
+      <c r="I730" s="2">
+        <v>41.728200000000001</v>
+      </c>
+      <c r="Q730" s="2" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="731" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B731" t="s">
+        <v>3122</v>
+      </c>
+      <c r="C731" t="s">
+        <v>852</v>
+      </c>
+      <c r="D731" t="s">
+        <v>3123</v>
+      </c>
+      <c r="G731" s="2" t="s">
+        <v>3117</v>
+      </c>
+      <c r="H731" s="12" t="s">
+        <v>3124</v>
+      </c>
+      <c r="I731" s="2">
+        <v>41.728200000000001</v>
+      </c>
+      <c r="Q731" s="2" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="732" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B732" t="s">
+        <v>3125</v>
+      </c>
+      <c r="C732" t="s">
+        <v>852</v>
+      </c>
+      <c r="D732" t="s">
+        <v>3126</v>
+      </c>
+      <c r="G732" s="2" t="s">
+        <v>3117</v>
+      </c>
+      <c r="H732" s="12" t="s">
+        <v>3124</v>
+      </c>
+      <c r="I732" s="2">
+        <v>41.728200000000001</v>
+      </c>
+      <c r="Q732" s="2" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="733" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B733" t="s">
+        <v>3127</v>
+      </c>
+      <c r="C733" t="s">
+        <v>858</v>
+      </c>
+      <c r="D733" t="s">
+        <v>3128</v>
+      </c>
+      <c r="G733" s="2" t="s">
+        <v>3129</v>
+      </c>
+      <c r="H733" s="12" t="s">
+        <v>3130</v>
+      </c>
+      <c r="I733" s="2">
+        <v>48.459000000000003</v>
+      </c>
+      <c r="Q733" s="2" t="s">
+        <v>3131</v>
+      </c>
+    </row>
+    <row r="734" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B734" t="s">
+        <v>859</v>
+      </c>
+      <c r="C734" t="s">
+        <v>860</v>
+      </c>
+      <c r="D734" t="s">
+        <v>3132</v>
+      </c>
+      <c r="G734" s="2" t="s">
+        <v>3129</v>
+      </c>
+      <c r="H734" s="12" t="s">
+        <v>3130</v>
+      </c>
+      <c r="I734" s="2">
+        <v>48.459000000000003</v>
+      </c>
+      <c r="Q734" s="2" t="s">
+        <v>3131</v>
+      </c>
+    </row>
+    <row r="735" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B735" t="s">
+        <v>861</v>
+      </c>
+      <c r="C735" t="s">
+        <v>862</v>
+      </c>
+      <c r="D735" t="s">
+        <v>3133</v>
+      </c>
+      <c r="G735" s="2" t="s">
+        <v>3129</v>
+      </c>
+      <c r="H735" s="12" t="s">
+        <v>3130</v>
+      </c>
+      <c r="I735" s="2">
+        <v>48.459000000000003</v>
+      </c>
+      <c r="Q735" s="2" t="s">
+        <v>3131</v>
+      </c>
+    </row>
+    <row r="736" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B736" t="s">
+        <v>863</v>
+      </c>
+      <c r="C736" t="s">
+        <v>864</v>
+      </c>
+      <c r="D736" t="s">
+        <v>3134</v>
+      </c>
+      <c r="G736" s="2" t="s">
+        <v>3129</v>
+      </c>
+      <c r="H736" s="12" t="s">
+        <v>3130</v>
+      </c>
+      <c r="I736" s="2">
+        <v>48.459000000000003</v>
+      </c>
+      <c r="Q736" s="2" t="s">
+        <v>3131</v>
+      </c>
+    </row>
+    <row r="737" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B737" t="s">
+        <v>3135</v>
+      </c>
+      <c r="C737" t="s">
+        <v>867</v>
+      </c>
+      <c r="D737" t="s">
+        <v>3136</v>
+      </c>
+      <c r="G737" s="2" t="s">
+        <v>3137</v>
+      </c>
+      <c r="H737" s="12" t="s">
+        <v>3138</v>
+      </c>
+      <c r="I737" s="2">
+        <v>55.012799999999999</v>
+      </c>
+      <c r="Q737" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="738" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B738" t="s">
+        <v>868</v>
+      </c>
+      <c r="C738" t="s">
+        <v>867</v>
+      </c>
+      <c r="D738" t="s">
+        <v>3139</v>
+      </c>
+      <c r="G738" s="2" t="s">
+        <v>3137</v>
+      </c>
+      <c r="H738" s="12" t="s">
+        <v>3138</v>
+      </c>
+      <c r="I738" s="2">
+        <v>55.012799999999999</v>
+      </c>
+      <c r="Q738" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="739" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B739" t="s">
+        <v>3140</v>
+      </c>
+      <c r="C739" t="s">
+        <v>871</v>
+      </c>
+      <c r="D739" t="s">
+        <v>3141</v>
+      </c>
+      <c r="G739" s="2" t="s">
+        <v>3142</v>
+      </c>
+      <c r="H739" s="12" t="s">
+        <v>3143</v>
+      </c>
+      <c r="I739" s="2">
+        <v>44.115400000000001</v>
+      </c>
+      <c r="Q739" s="2" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="740" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B740" t="s">
+        <v>3145</v>
+      </c>
+      <c r="C740" t="s">
+        <v>875</v>
+      </c>
+      <c r="D740" t="s">
+        <v>3146</v>
+      </c>
+      <c r="G740" s="2" t="s">
+        <v>3147</v>
+      </c>
+      <c r="H740" s="12" t="s">
+        <v>3148</v>
+      </c>
+      <c r="I740" s="2">
+        <v>40.482900000000001</v>
+      </c>
+      <c r="Q740" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="741" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B741" t="s">
+        <v>3149</v>
+      </c>
+      <c r="C741" t="s">
+        <v>458</v>
+      </c>
+      <c r="D741" t="s">
+        <v>3150</v>
+      </c>
+      <c r="G741" s="2" t="s">
+        <v>3147</v>
+      </c>
+      <c r="H741" s="12" t="s">
+        <v>3148</v>
+      </c>
+      <c r="I741" s="2">
+        <v>40.482900000000001</v>
+      </c>
+      <c r="Q741" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="742" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B742" t="s">
+        <v>3151</v>
+      </c>
+      <c r="C742" t="s">
+        <v>879</v>
+      </c>
+      <c r="D742" t="s">
+        <v>3152</v>
+      </c>
+      <c r="G742" s="2" t="s">
+        <v>3153</v>
+      </c>
+      <c r="H742" s="12" t="s">
+        <v>3154</v>
+      </c>
+      <c r="I742" s="2">
+        <v>33.351100000000002</v>
+      </c>
+      <c r="Q742" s="2" t="s">
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="743" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B743" t="s">
+        <v>3156</v>
+      </c>
+      <c r="C743" t="s">
+        <v>880</v>
+      </c>
+      <c r="D743" t="s">
+        <v>3157</v>
+      </c>
+      <c r="G743" s="2" t="s">
+        <v>3153</v>
+      </c>
+      <c r="H743" s="12" t="s">
+        <v>3158</v>
+      </c>
+      <c r="I743" s="2">
+        <v>33.351100000000002</v>
+      </c>
+      <c r="Q743" s="2" t="s">
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="744" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B744" t="s">
+        <v>408</v>
+      </c>
+      <c r="C744" t="s">
+        <v>376</v>
+      </c>
+      <c r="D744" t="s">
+        <v>3159</v>
+      </c>
+      <c r="G744" s="12" t="s">
+        <v>3160</v>
+      </c>
+      <c r="H744" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="I744" s="12">
+        <v>51.719299999999997</v>
+      </c>
+      <c r="L744" s="21"/>
+      <c r="Q744" s="12" t="s">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="746" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A746" s="2" t="s">
+        <v>3190</v>
+      </c>
+      <c r="B746" s="2">
+        <v>1</v>
+      </c>
+      <c r="C746" s="2" t="s">
+        <v>3162</v>
+      </c>
+      <c r="D746" s="2" t="s">
+        <v>3163</v>
+      </c>
+      <c r="E746" s="2" t="s">
+        <v>3164</v>
+      </c>
+      <c r="F746" s="2" t="s">
+        <v>3165</v>
+      </c>
+      <c r="G746" s="2" t="s">
+        <v>3166</v>
+      </c>
+      <c r="H746" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="I746" s="2">
+        <v>87.516000000000005</v>
+      </c>
+      <c r="K746" s="14" t="s">
+        <v>533</v>
+      </c>
+      <c r="L746" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="N746" s="2" t="s">
+        <v>3167</v>
+      </c>
+      <c r="O746" s="2" t="s">
+        <v>3168</v>
+      </c>
+      <c r="P746" s="2" t="s">
+        <v>3209</v>
+      </c>
+      <c r="S746" s="2" t="s">
+        <v>3169</v>
+      </c>
+    </row>
+    <row r="747" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B747" s="2">
+        <v>2</v>
+      </c>
+      <c r="C747" s="2" t="s">
+        <v>3170</v>
+      </c>
+      <c r="D747" s="2" t="s">
+        <v>3171</v>
+      </c>
+      <c r="E747" s="2" t="s">
+        <v>3172</v>
+      </c>
+      <c r="F747" s="2" t="s">
+        <v>3173</v>
+      </c>
+      <c r="G747" s="2" t="s">
+        <v>3174</v>
+      </c>
+      <c r="H747" s="2" t="s">
+        <v>3175</v>
+      </c>
+      <c r="I747" s="2">
+        <v>56.456000000000003</v>
+      </c>
+    </row>
+    <row r="748" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B748" s="2">
+        <v>3</v>
+      </c>
+      <c r="C748" s="2" t="s">
+        <v>3176</v>
+      </c>
+      <c r="D748" s="2" t="s">
+        <v>3208</v>
+      </c>
+      <c r="E748" s="2" t="s">
+        <v>3177</v>
+      </c>
+      <c r="F748" s="2" t="s">
+        <v>3178</v>
+      </c>
+      <c r="G748" s="2" t="s">
+        <v>3179</v>
+      </c>
+      <c r="H748" s="2" t="s">
+        <v>3175</v>
+      </c>
+      <c r="I748" s="2">
+        <v>59.454000000000001</v>
+      </c>
+    </row>
+    <row r="749" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B749" s="2">
+        <v>4</v>
+      </c>
+      <c r="C749" s="2" t="s">
+        <v>3180</v>
+      </c>
+      <c r="D749" s="2" t="s">
+        <v>3181</v>
+      </c>
+    </row>
+    <row r="750" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B750" s="2">
+        <v>5</v>
+      </c>
+      <c r="C750" s="2" t="s">
+        <v>3182</v>
+      </c>
+      <c r="D750" s="2" t="s">
+        <v>3183</v>
+      </c>
+    </row>
+    <row r="751" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B751" s="2">
+        <v>6</v>
+      </c>
+      <c r="C751" s="12" t="s">
+        <v>3184</v>
+      </c>
+      <c r="D751" s="12" t="s">
+        <v>3185</v>
+      </c>
+    </row>
+    <row r="752" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B752" s="2">
+        <v>7</v>
+      </c>
+      <c r="C752" s="12" t="s">
+        <v>3186</v>
+      </c>
+      <c r="D752" s="12" t="s">
+        <v>3187</v>
+      </c>
+    </row>
+    <row r="753" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B753" s="2">
+        <v>8</v>
+      </c>
+      <c r="C753" s="12" t="s">
+        <v>3188</v>
+      </c>
+      <c r="D753" s="12" t="s">
+        <v>3189</v>
       </c>
     </row>
   </sheetData>
@@ -31093,10 +33295,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D198"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="A190" sqref="A190:B198"/>
+    <sheetView topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="A202" sqref="A202:B207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -32691,6 +34893,78 @@
         <v>2946</v>
       </c>
     </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>3045</v>
+      </c>
+      <c r="B199" t="s">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>3047</v>
+      </c>
+      <c r="B200" t="s">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>3049</v>
+      </c>
+      <c r="B201" t="s">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>3192</v>
+      </c>
+      <c r="B202" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>3194</v>
+      </c>
+      <c r="B203" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>3196</v>
+      </c>
+      <c r="B204" t="s">
+        <v>3197</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>3198</v>
+      </c>
+      <c r="B205" t="s">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>3200</v>
+      </c>
+      <c r="B206" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>3202</v>
+      </c>
+      <c r="B207" t="s">
+        <v>3203</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32700,10 +34974,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -34212,6 +36486,62 @@
       </c>
       <c r="E106" t="s">
         <v>2929</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>3051</v>
+      </c>
+      <c r="B107" t="s">
+        <v>3052</v>
+      </c>
+      <c r="C107" t="s">
+        <v>3053</v>
+      </c>
+      <c r="E107" t="s">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>3192</v>
+      </c>
+      <c r="B108" t="s">
+        <v>3193</v>
+      </c>
+      <c r="C108" t="s">
+        <v>3204</v>
+      </c>
+      <c r="E108" t="s">
+        <v>3205</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>3196</v>
+      </c>
+      <c r="B109" t="s">
+        <v>3197</v>
+      </c>
+      <c r="C109" t="s">
+        <v>3206</v>
+      </c>
+      <c r="E109" t="s">
+        <v>3205</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>3202</v>
+      </c>
+      <c r="B110" t="s">
+        <v>3203</v>
+      </c>
+      <c r="C110" t="s">
+        <v>3207</v>
+      </c>
+      <c r="E110" t="s">
+        <v>3205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add new ecModel
</commit_message>
<xml_diff>
--- a/result_ecYeast/Data_Allchemicals.xlsx
+++ b/result_ecYeast/Data_Allchemicals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="3HP_Rxn " sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4317" uniqueCount="3210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4540" uniqueCount="3375">
   <si>
     <t>3-hydroxypropionate dehydrogenase</t>
   </si>
@@ -16451,6 +16451,905 @@
   <si>
     <t>glucose</t>
     <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>paclitaxel precursor</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taxadiene synthase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_0189 + 0.00173611 prot_Q2PRN4 -&gt; s_0633 + s_4412</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>TASY (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Taxus cuspidata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q2PRN4</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.3.17</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taxus brevifolia</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00034 mol/mol</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEP</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>glucose</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optimizing the biosynthesis of oxygenated and acetylated Taxol precursors in Saccharomyces cerevisiae using advanced bioprocessing strategies</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0904No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0019 + s_0434 + 4.08497e-05 prot_P24521  -&gt; s_0018 + s_0394 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.7.4.2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.8 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERG8</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0735No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0028 + s_0434 + 6.34194e-06 prot_P07277  -&gt; s_0019 + s_0394 + s_0794 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.7.1.36</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>43.8001 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERG12</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0028 + s_0539 + 6.34194e-06 prot_P07277  -&gt; s_0019 + s_0467 + s_0794 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0028 + s_0785 + 6.34194e-06 prot_P07277  -&gt; s_0019 + s_0739 + s_0794 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0028 + s_1559 + 6.34194e-06 prot_P07277  -&gt; s_0019 + s_0794 + s_1538 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0739No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0018 + s_0434 + 2.83447e-05 prot_P32377  -&gt; s_0394 + s_0456 + s_0943 + s_1322 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1.1.33</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.8 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERG19</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0355No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0943 + s_1376 + 0.000126263 prot_P08524  -&gt; s_0633 + s_0745 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5.1.1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0462No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0745 + s_0943 + 0.000126263 prot_P08524  -&gt; s_0190 + s_0633 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0667No1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0943 + 4.64511e-09 prot_P15496  -&gt; s_1376 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.3.3.2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>59800 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDI1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>r_0667_REVNo1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_1376 + 0.0022919 prot_P15496  -&gt; s_0943 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1212 (Kcat*2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>geranylgeranyl diphosphate synthase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_0190 + s_0943 + 3.30688e-05 prot_Q1L6K3 -&gt; s_0633 + s_0189</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q1L6K3</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5.1.29</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saccharomyces cerevisiae</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Acetyl-CoA acetyltransferase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_0373 + prot_Q9FD70 -&gt; s_0529 + s_0367</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>mvaE (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enterococcus faecalis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q9FD70</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3.1.9</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hydroxymethylglutaryl-CoA synthase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_0373 + s_0367 + s_0803 + 3.95132e-05 pprot_Q9FD71 -&gt; s_0218 + s_0529</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>mvaS (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enterococcus faecalis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q9FD71</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3.3.10</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taxadiene 5-alpha hydroxylase</t>
+  </si>
+  <si>
+    <t>s_4412 + s_1275 + prot_Q6WG30 -&gt; s_4413 + s_0803</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CYP725A4 (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Taxus cuspidata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q6WG30</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.14.99.37</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taxadien-5-alpha-ol O-acetyltransferase</t>
+  </si>
+  <si>
+    <t>s_4413 + s_0373 + 9.38756e-06 prot_Q9M6F0 -&gt; s_4414 + s_0529</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>TAT (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Taxus cuspidata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q9M6F0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3.1.162</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taxa-4(20),11(12)-dien-5alpha-yl acetate transport</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4414 -&gt; s_4415</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taxa-4(20),11(12)-dien-6alpha-yl acetate exchange</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4415 -&gt;</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q2PRN4</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>97.962 prot_pool  -&gt; prot_Q2PRN4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q1L6K3</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>42.153 prot_pool  -&gt; prot_Q1L6K3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q9FD70</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>86.497 prot_pool  -&gt; prot_Q9FD70</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q9FD71</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>42.151prot_pool  -&gt; prot_Q9FD71</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q6WG30</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>56.558 prot_pool  -&gt; prot_Q6WG30</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q9M6F0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>49.080 prot_pool  -&gt; prot_Q9M6F0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitamin A</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>geranylgeranyl diphosphate synthase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_0190 + s_0943 + 3.30688e-05 prot_Q1L6K3 -&gt; s_0633 + s_0189</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>crtE (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Xanthophyllomyces dendrorhous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00069 mol/mol</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00020 mol/mol</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>xylose</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALD6</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitamin A Production by Engineered Saccharomyces cerevisiae from Xylose via Two-Phase in Situ Extraction</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5.1.32</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.3.99.28</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q7Z858</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4238 + 0.000626472  prot_Q7Z859 -&gt; s_4239</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q7Z859</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.5.1.19</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beta-carotene 15,15'-dioxygenase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4239 + s_1275 + 0.00750751 prot_Q4PNI0 -&gt; 2 s_4416</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>blh (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Uncultured marine bacterium 66A03</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q4PNI0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.13.11.63</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>retinol dehydrogenase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4416 + s_1203 + s_0794 + prot_P00330 -&gt; s_4417 + s_1198</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADH (saccharomyces cerevisiae)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>P00330</t>
+  </si>
+  <si>
+    <t>1.1.1.1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>xylose reductase</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_0578 + s_0794 + s_1203 + 1.0101e-05 prot_P31867 -&gt; s_1566 + s_1198</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>XYL1 (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pichia stipitis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>P31867</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1.1.307</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_0578 + s_0794 + s_1212 + 1.0101e-05 prot_P31867 -&gt; s_1566 + s_1207</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_1566 + s_1198 + 9.15852e-06 prot_P22144 -&gt; s_0580 + s_0794 + s_1203</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>XYL2 (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pichia stipitis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>P22144</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1.1.9</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">s_0434 + s_0580 + 0.000242643 prot_Q9P938  -&gt; s_0394 + s_0581 + s_0794 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>XYL3 (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pichia stipitis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q9P938</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.7.1.17</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitamin A formation</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4416 + s_4417 -&gt; s_4418</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitamin A transport</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4418 -&gt; s_4419</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitamin A exchange</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4419 -&gt;</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q1L6K3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>42.153 prot_pool  -&gt; prot_Q1L6K3</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q7Z859</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>74.736 prot_pool  -&gt; prot_Q7Z859</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q7Z858</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>65.066 prot_pool  -&gt; prot_Q7Z858</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q4PNI0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>31.037 prot_pool  -&gt; prot_Q4PNI0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_P31867</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>35.923 prot_pool  -&gt; prot_P31867</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_P22144</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>38.521 prot_pool  -&gt; prot_P22144</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>draw_prot_Q9P938</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>69.397 prot_pool  -&gt; prot_Q9P938</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4412[c]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>taxadiene [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4413[c]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taxa-4(20),11-dien-5alpha-ol [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4414[c]</t>
+  </si>
+  <si>
+    <t>Taxa-4(20),11(12)-dien-5alpha-yl acetate [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4415[e]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taxa-4(20),11(12)-dien-6alpha-yl acetate [extracellular]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4416[c]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retinal [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4417[c]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retinol [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4418[c]</t>
+  </si>
+  <si>
+    <t>Vitamin A [cytoplasm]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_4419[e]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitamin A [extracellular]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecTaxadien_5alpha_yl_acetate.mat</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>heterogenous</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecVitamin_A.mat</t>
   </si>
 </sst>
 </file>
@@ -17033,7 +17932,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -18567,10 +19466,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T753"/>
+  <dimension ref="A1:T800"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F673" workbookViewId="0">
-      <selection activeCell="N706" sqref="N706"/>
+    <sheetView topLeftCell="A793" workbookViewId="0">
+      <selection activeCell="C810" sqref="C810"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -33271,7 +34170,7 @@
         <v>3187</v>
       </c>
     </row>
-    <row r="753" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="753" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B753" s="2">
         <v>8</v>
       </c>
@@ -33281,6 +34180,1029 @@
       <c r="D753" s="12" t="s">
         <v>3189</v>
       </c>
+    </row>
+    <row r="755" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A755" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="B755" s="2">
+        <v>1</v>
+      </c>
+      <c r="C755" s="2" t="s">
+        <v>3211</v>
+      </c>
+      <c r="D755" s="2" t="s">
+        <v>3212</v>
+      </c>
+      <c r="E755" s="2" t="s">
+        <v>3213</v>
+      </c>
+      <c r="F755" s="2" t="s">
+        <v>3214</v>
+      </c>
+      <c r="G755" s="2" t="s">
+        <v>3215</v>
+      </c>
+      <c r="H755" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="I755" s="2">
+        <v>97.962000000000003</v>
+      </c>
+      <c r="K755" s="14" t="s">
+        <v>3216</v>
+      </c>
+      <c r="L755" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="N755" s="2" t="s">
+        <v>3217</v>
+      </c>
+      <c r="O755" s="2" t="s">
+        <v>3218</v>
+      </c>
+      <c r="P755" s="2" t="s">
+        <v>3219</v>
+      </c>
+      <c r="S755" s="2" t="s">
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="756" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B756" t="s">
+        <v>3221</v>
+      </c>
+      <c r="C756" t="s">
+        <v>846</v>
+      </c>
+      <c r="D756" t="s">
+        <v>3222</v>
+      </c>
+      <c r="G756" s="2" t="s">
+        <v>3223</v>
+      </c>
+      <c r="H756" s="12" t="s">
+        <v>3224</v>
+      </c>
+      <c r="I756" s="2">
+        <v>50.4544</v>
+      </c>
+      <c r="Q756" s="2" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="757" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B757" t="s">
+        <v>3226</v>
+      </c>
+      <c r="C757" t="s">
+        <v>858</v>
+      </c>
+      <c r="D757" t="s">
+        <v>3227</v>
+      </c>
+      <c r="G757" s="2" t="s">
+        <v>3228</v>
+      </c>
+      <c r="H757" s="12" t="s">
+        <v>3229</v>
+      </c>
+      <c r="I757" s="2">
+        <v>48.459000000000003</v>
+      </c>
+      <c r="Q757" s="2" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="758" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B758" t="s">
+        <v>859</v>
+      </c>
+      <c r="C758" t="s">
+        <v>860</v>
+      </c>
+      <c r="D758" t="s">
+        <v>3231</v>
+      </c>
+      <c r="G758" s="2" t="s">
+        <v>3228</v>
+      </c>
+      <c r="H758" s="12" t="s">
+        <v>3229</v>
+      </c>
+      <c r="I758" s="2">
+        <v>48.459000000000003</v>
+      </c>
+      <c r="Q758" s="2" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="759" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B759" t="s">
+        <v>861</v>
+      </c>
+      <c r="C759" t="s">
+        <v>862</v>
+      </c>
+      <c r="D759" t="s">
+        <v>3232</v>
+      </c>
+      <c r="G759" s="2" t="s">
+        <v>3228</v>
+      </c>
+      <c r="H759" s="12" t="s">
+        <v>3229</v>
+      </c>
+      <c r="I759" s="2">
+        <v>48.459000000000003</v>
+      </c>
+      <c r="Q759" s="2" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="760" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B760" t="s">
+        <v>863</v>
+      </c>
+      <c r="C760" t="s">
+        <v>864</v>
+      </c>
+      <c r="D760" t="s">
+        <v>3233</v>
+      </c>
+      <c r="G760" s="2" t="s">
+        <v>3228</v>
+      </c>
+      <c r="H760" s="12" t="s">
+        <v>3229</v>
+      </c>
+      <c r="I760" s="2">
+        <v>48.459000000000003</v>
+      </c>
+      <c r="Q760" s="2" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="761" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B761" t="s">
+        <v>3234</v>
+      </c>
+      <c r="C761" t="s">
+        <v>871</v>
+      </c>
+      <c r="D761" t="s">
+        <v>3235</v>
+      </c>
+      <c r="G761" s="2" t="s">
+        <v>3236</v>
+      </c>
+      <c r="H761" s="12" t="s">
+        <v>3237</v>
+      </c>
+      <c r="I761" s="2">
+        <v>44.115400000000001</v>
+      </c>
+      <c r="Q761" s="2" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="762" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B762" t="s">
+        <v>3239</v>
+      </c>
+      <c r="C762" t="s">
+        <v>875</v>
+      </c>
+      <c r="D762" t="s">
+        <v>3240</v>
+      </c>
+      <c r="G762" s="2" t="s">
+        <v>3241</v>
+      </c>
+      <c r="H762" s="12" t="s">
+        <v>3242</v>
+      </c>
+      <c r="I762" s="2">
+        <v>40.482900000000001</v>
+      </c>
+      <c r="Q762" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="763" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B763" t="s">
+        <v>3243</v>
+      </c>
+      <c r="C763" t="s">
+        <v>458</v>
+      </c>
+      <c r="D763" t="s">
+        <v>3244</v>
+      </c>
+      <c r="G763" s="2" t="s">
+        <v>3241</v>
+      </c>
+      <c r="H763" s="12" t="s">
+        <v>3242</v>
+      </c>
+      <c r="I763" s="2">
+        <v>40.482900000000001</v>
+      </c>
+      <c r="Q763" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="764" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B764" t="s">
+        <v>3245</v>
+      </c>
+      <c r="C764" t="s">
+        <v>879</v>
+      </c>
+      <c r="D764" t="s">
+        <v>3246</v>
+      </c>
+      <c r="G764" s="2" t="s">
+        <v>3247</v>
+      </c>
+      <c r="H764" s="12" t="s">
+        <v>3248</v>
+      </c>
+      <c r="I764" s="2">
+        <v>33.351100000000002</v>
+      </c>
+      <c r="Q764" s="2" t="s">
+        <v>3249</v>
+      </c>
+    </row>
+    <row r="765" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B765" t="s">
+        <v>3250</v>
+      </c>
+      <c r="C765" t="s">
+        <v>880</v>
+      </c>
+      <c r="D765" t="s">
+        <v>3251</v>
+      </c>
+      <c r="G765" s="2" t="s">
+        <v>3247</v>
+      </c>
+      <c r="H765" s="12" t="s">
+        <v>3252</v>
+      </c>
+      <c r="I765" s="2">
+        <v>33.351100000000002</v>
+      </c>
+      <c r="Q765" s="2" t="s">
+        <v>3249</v>
+      </c>
+    </row>
+    <row r="766" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B766" s="2">
+        <v>2</v>
+      </c>
+      <c r="C766" s="12" t="s">
+        <v>3253</v>
+      </c>
+      <c r="D766" s="12" t="s">
+        <v>3254</v>
+      </c>
+      <c r="E766" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="F766" s="12" t="s">
+        <v>3255</v>
+      </c>
+      <c r="G766" s="12" t="s">
+        <v>3256</v>
+      </c>
+      <c r="H766" s="12">
+        <v>8.4</v>
+      </c>
+      <c r="I766" s="12">
+        <v>42.152999999999999</v>
+      </c>
+      <c r="J766" s="12"/>
+      <c r="K766" s="14" t="s">
+        <v>3257</v>
+      </c>
+    </row>
+    <row r="767" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B767" s="2">
+        <v>3</v>
+      </c>
+      <c r="C767" s="12" t="s">
+        <v>3258</v>
+      </c>
+      <c r="D767" s="12" t="s">
+        <v>3259</v>
+      </c>
+      <c r="E767" s="2" t="s">
+        <v>3260</v>
+      </c>
+      <c r="F767" s="2" t="s">
+        <v>3261</v>
+      </c>
+      <c r="G767" s="2" t="s">
+        <v>3262</v>
+      </c>
+      <c r="H767" s="2" t="s">
+        <v>3263</v>
+      </c>
+      <c r="I767" s="12">
+        <v>86.497</v>
+      </c>
+    </row>
+    <row r="768" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B768" s="2">
+        <v>4</v>
+      </c>
+      <c r="C768" s="12" t="s">
+        <v>3264</v>
+      </c>
+      <c r="D768" s="12" t="s">
+        <v>3265</v>
+      </c>
+      <c r="E768" s="2" t="s">
+        <v>3266</v>
+      </c>
+      <c r="F768" s="2" t="s">
+        <v>3267</v>
+      </c>
+      <c r="G768" s="2" t="s">
+        <v>3268</v>
+      </c>
+      <c r="H768" s="2">
+        <v>7.0251666666666672</v>
+      </c>
+      <c r="I768" s="12">
+        <v>42.151000000000003</v>
+      </c>
+      <c r="J768" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="769" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B769" s="2">
+        <v>5</v>
+      </c>
+      <c r="C769" s="2" t="s">
+        <v>3269</v>
+      </c>
+      <c r="D769" s="2" t="s">
+        <v>3270</v>
+      </c>
+      <c r="E769" s="2" t="s">
+        <v>3271</v>
+      </c>
+      <c r="F769" s="2" t="s">
+        <v>3272</v>
+      </c>
+      <c r="G769" s="2" t="s">
+        <v>3273</v>
+      </c>
+      <c r="H769" s="2" t="s">
+        <v>3263</v>
+      </c>
+      <c r="I769" s="12">
+        <v>56.558</v>
+      </c>
+    </row>
+    <row r="770" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B770" s="2">
+        <v>6</v>
+      </c>
+      <c r="C770" s="2" t="s">
+        <v>3274</v>
+      </c>
+      <c r="D770" s="2" t="s">
+        <v>3275</v>
+      </c>
+      <c r="E770" s="2" t="s">
+        <v>3276</v>
+      </c>
+      <c r="F770" s="2" t="s">
+        <v>3277</v>
+      </c>
+      <c r="G770" s="2" t="s">
+        <v>3278</v>
+      </c>
+      <c r="H770" s="2">
+        <v>29.59</v>
+      </c>
+      <c r="I770" s="12">
+        <v>49.08</v>
+      </c>
+    </row>
+    <row r="771" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B771" s="2">
+        <v>7</v>
+      </c>
+      <c r="C771" s="2" t="s">
+        <v>3279</v>
+      </c>
+      <c r="D771" s="2" t="s">
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="772" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B772" s="2">
+        <v>8</v>
+      </c>
+      <c r="C772" s="2" t="s">
+        <v>3281</v>
+      </c>
+      <c r="D772" s="2" t="s">
+        <v>3282</v>
+      </c>
+    </row>
+    <row r="773" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B773" s="2">
+        <v>9</v>
+      </c>
+      <c r="C773" s="12" t="s">
+        <v>3283</v>
+      </c>
+      <c r="D773" s="12" t="s">
+        <v>3284</v>
+      </c>
+    </row>
+    <row r="774" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B774" s="2">
+        <v>10</v>
+      </c>
+      <c r="C774" s="12" t="s">
+        <v>3285</v>
+      </c>
+      <c r="D774" s="12" t="s">
+        <v>3286</v>
+      </c>
+    </row>
+    <row r="775" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B775" s="2">
+        <v>11</v>
+      </c>
+      <c r="C775" s="12" t="s">
+        <v>3287</v>
+      </c>
+      <c r="D775" s="12" t="s">
+        <v>3288</v>
+      </c>
+    </row>
+    <row r="776" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B776" s="2">
+        <v>12</v>
+      </c>
+      <c r="C776" s="12" t="s">
+        <v>3289</v>
+      </c>
+      <c r="D776" s="12" t="s">
+        <v>3290</v>
+      </c>
+    </row>
+    <row r="777" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B777" s="2">
+        <v>13</v>
+      </c>
+      <c r="C777" s="12" t="s">
+        <v>3291</v>
+      </c>
+      <c r="D777" s="12" t="s">
+        <v>3292</v>
+      </c>
+    </row>
+    <row r="778" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B778" s="2">
+        <v>14</v>
+      </c>
+      <c r="C778" s="12" t="s">
+        <v>3293</v>
+      </c>
+      <c r="D778" s="12" t="s">
+        <v>3294</v>
+      </c>
+    </row>
+    <row r="780" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A780" s="2" t="s">
+        <v>3295</v>
+      </c>
+      <c r="B780" s="12">
+        <v>1</v>
+      </c>
+      <c r="C780" s="12" t="s">
+        <v>3296</v>
+      </c>
+      <c r="D780" s="12" t="s">
+        <v>3297</v>
+      </c>
+      <c r="E780" s="12" t="s">
+        <v>3298</v>
+      </c>
+      <c r="F780" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="G780" s="12" t="s">
+        <v>3256</v>
+      </c>
+      <c r="H780" s="12">
+        <v>8.4</v>
+      </c>
+      <c r="I780" s="12">
+        <v>42.152999999999999</v>
+      </c>
+      <c r="J780" s="12"/>
+      <c r="K780" s="14" t="s">
+        <v>3257</v>
+      </c>
+      <c r="L780" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="M780" s="2" t="s">
+        <v>3299</v>
+      </c>
+      <c r="N780" s="2" t="s">
+        <v>3300</v>
+      </c>
+      <c r="O780" s="2" t="s">
+        <v>3301</v>
+      </c>
+      <c r="P780" s="2" t="s">
+        <v>3302</v>
+      </c>
+      <c r="R780" s="2" t="s">
+        <v>3303</v>
+      </c>
+      <c r="S780" s="2" t="s">
+        <v>3304</v>
+      </c>
+    </row>
+    <row r="781" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B781" s="12">
+        <v>2</v>
+      </c>
+      <c r="C781" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="D781" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="E781" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="F781" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="G781" s="12" t="s">
+        <v>3305</v>
+      </c>
+      <c r="H781" s="12">
+        <v>8.3455200000000007E-2</v>
+      </c>
+      <c r="I781" s="12">
+        <v>74.736000000000004</v>
+      </c>
+      <c r="J781" s="12">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="K781" s="12"/>
+    </row>
+    <row r="782" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B782" s="12">
+        <v>3</v>
+      </c>
+      <c r="C782" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="D782" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="E782" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="F782" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="G782" s="12" t="s">
+        <v>3306</v>
+      </c>
+      <c r="H782" s="12">
+        <v>3.1448566666666668E-4</v>
+      </c>
+      <c r="I782" s="12">
+        <v>65.066000000000003</v>
+      </c>
+      <c r="J782" s="12">
+        <v>2.9E-4</v>
+      </c>
+      <c r="K782" s="12"/>
+    </row>
+    <row r="783" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B783" s="12">
+        <v>4</v>
+      </c>
+      <c r="C783" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="D783" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="E783" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="F783" s="12" t="s">
+        <v>3307</v>
+      </c>
+      <c r="G783" s="12" t="s">
+        <v>3306</v>
+      </c>
+      <c r="H783" s="12">
+        <v>3.1448566666666668E-4</v>
+      </c>
+      <c r="I783" s="12">
+        <v>65.066000000000003</v>
+      </c>
+      <c r="J783" s="12">
+        <v>2.9E-4</v>
+      </c>
+      <c r="K783" s="12"/>
+    </row>
+    <row r="784" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B784" s="12">
+        <v>5</v>
+      </c>
+      <c r="C784" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="D784" s="12" t="s">
+        <v>3308</v>
+      </c>
+      <c r="E784" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="F784" s="12" t="s">
+        <v>3309</v>
+      </c>
+      <c r="G784" s="12" t="s">
+        <v>3310</v>
+      </c>
+      <c r="H784" s="12">
+        <v>0.44343359999999998</v>
+      </c>
+      <c r="I784" s="12">
+        <v>74.736000000000004</v>
+      </c>
+      <c r="J784" s="12">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="K784" s="12"/>
+    </row>
+    <row r="785" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B785" s="12">
+        <v>6</v>
+      </c>
+      <c r="C785" s="12" t="s">
+        <v>3311</v>
+      </c>
+      <c r="D785" s="12" t="s">
+        <v>3312</v>
+      </c>
+      <c r="E785" s="12" t="s">
+        <v>3313</v>
+      </c>
+      <c r="F785" s="2" t="s">
+        <v>3314</v>
+      </c>
+      <c r="G785" s="2" t="s">
+        <v>3315</v>
+      </c>
+      <c r="H785" s="12">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I785" s="12">
+        <v>31.036999999999999</v>
+      </c>
+    </row>
+    <row r="786" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B786" s="12">
+        <v>7</v>
+      </c>
+      <c r="C786" s="11" t="s">
+        <v>3316</v>
+      </c>
+      <c r="D786" s="2" t="s">
+        <v>3317</v>
+      </c>
+      <c r="E786" s="12" t="s">
+        <v>3318</v>
+      </c>
+      <c r="F786" s="2" t="s">
+        <v>3319</v>
+      </c>
+      <c r="G786" s="2" t="s">
+        <v>3320</v>
+      </c>
+      <c r="H786" s="2" t="s">
+        <v>3321</v>
+      </c>
+      <c r="I786" s="12">
+        <v>36.848700000000001</v>
+      </c>
+    </row>
+    <row r="787" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A787" s="16"/>
+      <c r="B787" s="12">
+        <v>8</v>
+      </c>
+      <c r="C787" s="12" t="s">
+        <v>3322</v>
+      </c>
+      <c r="D787" s="12" t="s">
+        <v>3323</v>
+      </c>
+      <c r="E787" s="12" t="s">
+        <v>3324</v>
+      </c>
+      <c r="F787" s="12" t="s">
+        <v>3325</v>
+      </c>
+      <c r="G787" s="12" t="s">
+        <v>3326</v>
+      </c>
+      <c r="H787" s="12">
+        <v>27.5</v>
+      </c>
+      <c r="I787" s="12">
+        <v>35.923000000000002</v>
+      </c>
+      <c r="L787" s="21"/>
+    </row>
+    <row r="788" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A788" s="16"/>
+      <c r="B788" s="12">
+        <v>9</v>
+      </c>
+      <c r="C788" s="12" t="s">
+        <v>3322</v>
+      </c>
+      <c r="D788" s="12" t="s">
+        <v>3327</v>
+      </c>
+      <c r="E788" s="12" t="s">
+        <v>3324</v>
+      </c>
+      <c r="F788" s="12" t="s">
+        <v>2905</v>
+      </c>
+      <c r="G788" s="12" t="s">
+        <v>3326</v>
+      </c>
+      <c r="H788" s="12">
+        <v>27.5</v>
+      </c>
+      <c r="I788" s="12">
+        <v>35.923000000000002</v>
+      </c>
+      <c r="L788" s="21"/>
+    </row>
+    <row r="789" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A789" s="16"/>
+      <c r="B789" s="12">
+        <v>10</v>
+      </c>
+      <c r="C789" s="12" t="s">
+        <v>2906</v>
+      </c>
+      <c r="D789" s="12" t="s">
+        <v>3328</v>
+      </c>
+      <c r="E789" s="12" t="s">
+        <v>3329</v>
+      </c>
+      <c r="F789" s="12" t="s">
+        <v>3330</v>
+      </c>
+      <c r="G789" s="12" t="s">
+        <v>3331</v>
+      </c>
+      <c r="H789" s="12">
+        <v>30.33</v>
+      </c>
+      <c r="I789" s="12">
+        <v>38.521000000000001</v>
+      </c>
+      <c r="L789" s="21"/>
+    </row>
+    <row r="790" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A790" s="16"/>
+      <c r="B790" s="12">
+        <v>11</v>
+      </c>
+      <c r="C790" s="12" t="s">
+        <v>2911</v>
+      </c>
+      <c r="D790" s="12" t="s">
+        <v>3332</v>
+      </c>
+      <c r="E790" s="12" t="s">
+        <v>3333</v>
+      </c>
+      <c r="F790" s="2" t="s">
+        <v>3334</v>
+      </c>
+      <c r="G790" s="2" t="s">
+        <v>3335</v>
+      </c>
+      <c r="H790" s="2">
+        <v>1.1448191766666667</v>
+      </c>
+      <c r="I790" s="2">
+        <v>69.397000000000006</v>
+      </c>
+      <c r="J790" s="2">
+        <v>0.98980000000000001</v>
+      </c>
+      <c r="L790" s="21"/>
+    </row>
+    <row r="791" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A791" s="16"/>
+      <c r="B791" s="12">
+        <v>12</v>
+      </c>
+      <c r="C791" s="12" t="s">
+        <v>3336</v>
+      </c>
+      <c r="D791" s="12" t="s">
+        <v>3337</v>
+      </c>
+      <c r="F791" s="2"/>
+      <c r="G791" s="2"/>
+      <c r="H791" s="2"/>
+      <c r="I791" s="2"/>
+      <c r="J791" s="2"/>
+      <c r="L791" s="21"/>
+    </row>
+    <row r="792" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A792" s="16"/>
+      <c r="B792" s="12">
+        <v>13</v>
+      </c>
+      <c r="C792" s="12" t="s">
+        <v>3338</v>
+      </c>
+      <c r="D792" s="12" t="s">
+        <v>3339</v>
+      </c>
+      <c r="F792" s="2"/>
+      <c r="G792" s="2"/>
+      <c r="H792" s="2"/>
+      <c r="I792" s="2"/>
+      <c r="J792" s="2"/>
+      <c r="L792" s="21"/>
+    </row>
+    <row r="793" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A793" s="16"/>
+      <c r="B793" s="12">
+        <v>14</v>
+      </c>
+      <c r="C793" s="12" t="s">
+        <v>3340</v>
+      </c>
+      <c r="D793" s="12" t="s">
+        <v>3341</v>
+      </c>
+      <c r="F793" s="2"/>
+      <c r="G793" s="2"/>
+      <c r="H793" s="2"/>
+      <c r="I793" s="2"/>
+      <c r="J793" s="2"/>
+      <c r="L793" s="21"/>
+    </row>
+    <row r="794" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A794" s="16"/>
+      <c r="B794" s="12">
+        <v>15</v>
+      </c>
+      <c r="C794" s="12" t="s">
+        <v>3342</v>
+      </c>
+      <c r="D794" s="12" t="s">
+        <v>3343</v>
+      </c>
+      <c r="F794" s="2"/>
+      <c r="G794" s="2"/>
+      <c r="H794" s="2"/>
+      <c r="I794" s="2"/>
+      <c r="J794" s="2"/>
+      <c r="L794" s="21"/>
+    </row>
+    <row r="795" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A795" s="16"/>
+      <c r="B795" s="12">
+        <v>16</v>
+      </c>
+      <c r="C795" s="12" t="s">
+        <v>3344</v>
+      </c>
+      <c r="D795" s="12" t="s">
+        <v>3345</v>
+      </c>
+      <c r="F795" s="2"/>
+      <c r="G795" s="2"/>
+      <c r="H795" s="2"/>
+      <c r="I795" s="2"/>
+      <c r="J795" s="2"/>
+      <c r="L795" s="21"/>
+    </row>
+    <row r="796" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A796" s="16"/>
+      <c r="B796" s="12">
+        <v>17</v>
+      </c>
+      <c r="C796" s="12" t="s">
+        <v>3346</v>
+      </c>
+      <c r="D796" s="12" t="s">
+        <v>3347</v>
+      </c>
+      <c r="F796" s="2"/>
+      <c r="G796" s="2"/>
+      <c r="H796" s="2"/>
+      <c r="I796" s="2"/>
+      <c r="J796" s="2"/>
+      <c r="L796" s="21"/>
+    </row>
+    <row r="797" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A797" s="16"/>
+      <c r="B797" s="12">
+        <v>18</v>
+      </c>
+      <c r="C797" s="12" t="s">
+        <v>3348</v>
+      </c>
+      <c r="D797" s="12" t="s">
+        <v>3349</v>
+      </c>
+      <c r="F797" s="2"/>
+      <c r="G797" s="2"/>
+      <c r="H797" s="2"/>
+      <c r="I797" s="2"/>
+      <c r="J797" s="2"/>
+      <c r="L797" s="21"/>
+    </row>
+    <row r="798" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A798" s="16"/>
+      <c r="B798" s="12">
+        <v>19</v>
+      </c>
+      <c r="C798" s="12" t="s">
+        <v>3350</v>
+      </c>
+      <c r="D798" s="12" t="s">
+        <v>3351</v>
+      </c>
+      <c r="F798" s="2"/>
+      <c r="G798" s="2"/>
+      <c r="H798" s="2"/>
+      <c r="I798" s="2"/>
+      <c r="J798" s="2"/>
+      <c r="L798" s="21"/>
+    </row>
+    <row r="799" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A799" s="16"/>
+      <c r="B799" s="12">
+        <v>20</v>
+      </c>
+      <c r="C799" s="12" t="s">
+        <v>3352</v>
+      </c>
+      <c r="D799" s="12" t="s">
+        <v>3353</v>
+      </c>
+      <c r="F799" s="2"/>
+      <c r="G799" s="2"/>
+      <c r="H799" s="2"/>
+      <c r="I799" s="2"/>
+      <c r="J799" s="2"/>
+      <c r="L799" s="21"/>
+    </row>
+    <row r="800" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A800" s="16"/>
+      <c r="B800" s="12">
+        <v>21</v>
+      </c>
+      <c r="C800" s="12" t="s">
+        <v>3354</v>
+      </c>
+      <c r="D800" s="12" t="s">
+        <v>3355</v>
+      </c>
+      <c r="F800" s="2"/>
+      <c r="G800" s="2"/>
+      <c r="H800" s="2"/>
+      <c r="I800" s="2"/>
+      <c r="J800" s="2"/>
+      <c r="L800" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -33295,10 +35217,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:D215"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202:B207"/>
+    <sheetView topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -34965,6 +36887,70 @@
         <v>3203</v>
       </c>
     </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>3356</v>
+      </c>
+      <c r="B208" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>3358</v>
+      </c>
+      <c r="B209" t="s">
+        <v>3359</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>3360</v>
+      </c>
+      <c r="B210" t="s">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>3362</v>
+      </c>
+      <c r="B211" t="s">
+        <v>3363</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>3364</v>
+      </c>
+      <c r="B212" t="s">
+        <v>3365</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>3366</v>
+      </c>
+      <c r="B213" t="s">
+        <v>3367</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>3368</v>
+      </c>
+      <c r="B214" t="s">
+        <v>3369</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>3370</v>
+      </c>
+      <c r="B215" t="s">
+        <v>3371</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34974,10 +36960,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -36542,6 +38528,34 @@
       </c>
       <c r="E110" t="s">
         <v>3205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>3362</v>
+      </c>
+      <c r="B111" t="s">
+        <v>3363</v>
+      </c>
+      <c r="C111" t="s">
+        <v>3372</v>
+      </c>
+      <c r="E111" t="s">
+        <v>3373</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>3370</v>
+      </c>
+      <c r="B112" t="s">
+        <v>3371</v>
+      </c>
+      <c r="C112" t="s">
+        <v>3374</v>
+      </c>
+      <c r="E112" t="s">
+        <v>3373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>